<commit_message>
Implement spreadsheet parsing submodules in main script
Updated command for running it:

 python scripts/add_new_species.py --user_form=blahblah --user_spreadsheet=scripts/add_new_species/tests/fixtures/submission_form_example/02-Data_Tracks_Form_v1.1.0_fix.xlsx --species_image=scripts/add_new_species/tests/fixtures/example_images/image_4_3.png --overwrite

See e5ccd2c commit message for docker command
</commit_message>
<xml_diff>
--- a/scripts/add_new_species/tests/fixtures/submission_form_example/02-Data_Tracks_Form_v1.1.0_fix.xlsx
+++ b/scripts/add_new_species/tests/fixtures/submission_form_example/02-Data_Tracks_Form_v1.1.0_fix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danbr757/Github/genome-portal/tests/fixtures/submission_form_example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danbr757/Github/genome-portal/scripts/add_new_species/tests/fixtures/submission_form_example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FB81E4-6985-A141-AB4B-BB7D529C2005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D742BC-75F9-E845-8B09-F88067936223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
@@ -61,9 +61,6 @@
     <t>doi_link_to_repository</t>
   </si>
   <si>
-    <t>GCA_900323705.1</t>
-  </si>
-  <si>
     <t>CAVLGL01.fasta.gz</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>https://ftp.ebi.ac.uk/pub/databases/ena/wgs/public/cav/CAVLGL01.fasta.gz</t>
+  </si>
+  <si>
+    <t>GCA_963668995.1</t>
   </si>
 </sst>
 </file>
@@ -551,7 +551,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,7 +587,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>12</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -613,22 +613,22 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>3</v>
@@ -637,31 +637,31 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>3</v>
@@ -670,28 +670,28 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>3</v>
@@ -700,28 +700,28 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>3</v>
@@ -730,28 +730,28 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>3</v>
@@ -760,28 +760,28 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>3</v>
@@ -790,28 +790,28 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>3</v>
@@ -820,10 +820,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>